<commit_message>
add test rail result
</commit_message>
<xml_diff>
--- a/Test Case/Test Cases.xlsx
+++ b/Test Case/Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapdi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapdi\Code\qa-testing-portfolio\Test Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFECB3E-9DE7-4B96-B7A7-A6D180E704FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0671506D-B543-4896-97E7-612A27BE25B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,8 +30,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>Website</t>
   </si>
@@ -186,9 +208,6 @@
   <si>
     <t>1. Failed login
 2. System displayed error message</t>
-  </si>
-  <si>
-    <t>Not tested</t>
   </si>
   <si>
     <t>Login-004</t>
@@ -518,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -577,6 +596,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -589,13 +617,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1174,9 +1196,9 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1215,7 @@
     <col min="12" max="12" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1215,7 +1237,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1230,14 +1252,14 @@
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="10">
-        <f>SUMPRODUCT((K10:K11="Passed") + (K10:K11="Failed"))</f>
-        <v>1</v>
+      <c r="I2" s="10" cm="1">
+        <f t="array" ref="I2">SUMPRODUCT((K10:K16="Passed") + (K10:K16="Failed"))</f>
+        <v>7</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1254,39 +1276,39 @@
       </c>
       <c r="I3" s="10">
         <f>COUNTIF(K10:K16, "Not tested")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="26"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="14" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="15">
-        <f>COUNTIF(K10:K11, "Passed")</f>
-        <v>1</v>
+        <f>COUNTIF(K10:K16, "Passed")</f>
+        <v>7</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+    <row r="5" spans="1:12" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="27"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="16" t="s">
         <v>10</v>
       </c>
@@ -1297,7 +1319,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1310,7 +1332,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1323,7 +1345,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -1375,22 +1397,22 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="55.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="23" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="33" t="s">
         <v>27</v>
       </c>
       <c r="G10" s="22" t="s">
@@ -1405,20 +1427,20 @@
       <c r="J10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="31"/>
+      <c r="L10" s="24"/>
     </row>
     <row r="11" spans="1:12" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="23" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="21" t="s">
@@ -1439,33 +1461,33 @@
       <c r="J11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="31"/>
+      <c r="K11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>43</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>44</v>
       </c>
       <c r="I12" s="21" t="s">
         <v>38</v>
@@ -1473,30 +1495,30 @@
       <c r="J12" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="31"/>
+      <c r="K12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="G13" s="22" t="s">
         <v>47</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>48</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21" t="s">
@@ -1505,33 +1527,33 @@
       <c r="J13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="31"/>
+      <c r="K13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="32"/>
+      <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="F14" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="G14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="H14" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>53</v>
       </c>
       <c r="I14" s="21" t="s">
         <v>38</v>
@@ -1539,33 +1561,33 @@
       <c r="J14" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="31"/>
+      <c r="K14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="24"/>
     </row>
     <row r="15" spans="1:12" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="F15" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>57</v>
       </c>
       <c r="I15" s="21" t="s">
         <v>38</v>
@@ -1573,42 +1595,42 @@
       <c r="J15" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="31"/>
+      <c r="K15" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="24"/>
     </row>
     <row r="16" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="30" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="F16" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="22" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K16" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" s="31"/>
+        <v>60</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L16" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>